<commit_message>
Functional GUI with economic results
</commit_message>
<xml_diff>
--- a/Engine/results.xlsx
+++ b/Engine/results.xlsx
@@ -405,1523 +405,1523 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>3810756.78093064</v>
+        <v>4110954.86224926</v>
       </c>
       <c r="B2">
-        <v>1480</v>
+        <v>2888</v>
       </c>
       <c r="C2">
-        <v>792.701735989073</v>
+        <v>674.823877519005</v>
       </c>
       <c r="D2">
-        <v>4742.9665155198</v>
+        <v>8051.78188275135</v>
       </c>
       <c r="E2">
-        <v>0.285402434006795</v>
+        <v>0.897011196648189</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>3847352.9440034</v>
+        <v>4123396.76341082</v>
       </c>
       <c r="B3">
-        <v>1480</v>
+        <v>2894</v>
       </c>
       <c r="C3">
-        <v>770.985629210649</v>
+        <v>674.823877519005</v>
       </c>
       <c r="D3">
-        <v>4941.21253603673</v>
+        <v>7842.24562486707</v>
       </c>
       <c r="E3">
-        <v>0.282970421877938</v>
+        <v>0.904076753785699</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
-        <v>3851140.48081272</v>
+        <v>4142553.83019822</v>
       </c>
       <c r="B4">
-        <v>1480</v>
+        <v>2888</v>
       </c>
       <c r="C4">
-        <v>849.722587024833</v>
+        <v>606.683782207199</v>
       </c>
       <c r="D4">
-        <v>4941.21253603673</v>
+        <v>8622.15365956532</v>
       </c>
       <c r="E4">
-        <v>0.330170422730092</v>
+        <v>0.772607919248676</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1">
-        <v>3858697.99543544</v>
+        <v>4146397.65588329</v>
       </c>
       <c r="B5">
-        <v>1617</v>
+        <v>2981</v>
       </c>
       <c r="C5">
-        <v>739.507967920055</v>
+        <v>674.823877519005</v>
       </c>
       <c r="D5">
-        <v>4941.21253603673</v>
+        <v>8051.78188275135</v>
       </c>
       <c r="E5">
-        <v>0.295112411841623</v>
+        <v>1.00197768798684</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1">
-        <v>3868704.60901371</v>
+        <v>4154681.16270219</v>
       </c>
       <c r="B6">
-        <v>1608</v>
+        <v>2888</v>
       </c>
       <c r="C6">
-        <v>752.33164005286</v>
+        <v>627.686692429166</v>
       </c>
       <c r="D6">
-        <v>4588.43844529101</v>
+        <v>7975.84177056508</v>
       </c>
       <c r="E6">
-        <v>0.287278642971784</v>
+        <v>0.80427876489639</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1">
-        <v>3875632.00742305</v>
+        <v>4176620.82092099</v>
       </c>
       <c r="B7">
-        <v>1480</v>
+        <v>2873</v>
       </c>
       <c r="C7">
-        <v>887.678195705465</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D7">
-        <v>4941.21253603673</v>
+        <v>8734.87906408344</v>
       </c>
       <c r="E7">
-        <v>0.359357499346237</v>
+        <v>0.701382144029363</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
-        <v>3877679.69610705</v>
+        <v>4180581.52881229</v>
       </c>
       <c r="B8">
-        <v>1480</v>
+        <v>2873</v>
       </c>
       <c r="C8">
-        <v>793.108304608571</v>
+        <v>639.670597771826</v>
       </c>
       <c r="D8">
-        <v>3868.66391509577</v>
+        <v>9743.01363669133</v>
       </c>
       <c r="E8">
-        <v>0.254751267683134</v>
+        <v>0.834582719602757</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">
-        <v>3880692.95595834</v>
+        <v>4213186.34982211</v>
       </c>
       <c r="B9">
-        <v>1340</v>
+        <v>2971</v>
       </c>
       <c r="C9">
-        <v>887.678195705465</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D9">
-        <v>3724.88061318363</v>
+        <v>9625.96539612402</v>
       </c>
       <c r="E9">
-        <v>0.270474055726732</v>
+        <v>0.779521110382623</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
-        <v>3883061.62912319</v>
+        <v>4218176.45323407</v>
       </c>
       <c r="B10">
-        <v>1480</v>
+        <v>2888</v>
       </c>
       <c r="C10">
-        <v>887.678195705465</v>
+        <v>674.823877519005</v>
       </c>
       <c r="D10">
-        <v>5099.4102571827</v>
+        <v>7019.22998449514</v>
       </c>
       <c r="E10">
-        <v>0.366212709371976</v>
+        <v>0.908157177118328</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
-        <v>3899346.5600161</v>
+        <v>4225403.47019635</v>
       </c>
       <c r="B11">
-        <v>1480</v>
+        <v>2971</v>
       </c>
       <c r="C11">
-        <v>887.678195705465</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D11">
-        <v>5301.68396185874</v>
+        <v>10068.8735503158</v>
       </c>
       <c r="E11">
-        <v>0.373353473844784</v>
+        <v>0.78241665718034</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
-        <v>3901321.20645691</v>
+        <v>4229591.5314428</v>
       </c>
       <c r="B12">
-        <v>1480</v>
+        <v>2856</v>
       </c>
       <c r="C12">
-        <v>857.209795921401</v>
+        <v>712.877911029973</v>
       </c>
       <c r="D12">
-        <v>3294.94655338834</v>
+        <v>8350.6339821697</v>
       </c>
       <c r="E12">
-        <v>0.258073032726675</v>
+        <v>1.04742238446377</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1">
-        <v>3901578.60885041</v>
+        <v>4231159.33438104</v>
       </c>
       <c r="B13">
-        <v>1348</v>
+        <v>3040</v>
       </c>
       <c r="C13">
-        <v>887.678195705465</v>
+        <v>553.654169070104</v>
       </c>
       <c r="D13">
-        <v>3157.23657818223</v>
+        <v>8734.87906408344</v>
       </c>
       <c r="E13">
-        <v>0.242792022341999</v>
+        <v>0.789461349549274</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1">
-        <v>3907017.74415671</v>
+        <v>4240294.9821661</v>
       </c>
       <c r="B14">
-        <v>1586</v>
+        <v>3112</v>
       </c>
       <c r="C14">
-        <v>880.237039508552</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D14">
-        <v>5093.20344861765</v>
+        <v>9847.72679625696</v>
       </c>
       <c r="E14">
-        <v>0.392446257079999</v>
+        <v>0.880628966635406</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
-        <v>3921697.88414204</v>
+        <v>4244856.40611595</v>
       </c>
       <c r="B15">
-        <v>1480</v>
+        <v>2873</v>
       </c>
       <c r="C15">
-        <v>736.967708253454</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D15">
-        <v>4242.00555134723</v>
+        <v>7449.00079265366</v>
       </c>
       <c r="E15">
-        <v>0.246854261138953</v>
+        <v>0.696896344685754</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
-        <v>3944412.28722</v>
+        <v>4326045.23874566</v>
       </c>
       <c r="B16">
-        <v>1435</v>
+        <v>3367</v>
       </c>
       <c r="C16">
-        <v>887.678195705465</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D16">
-        <v>5757.65651580115</v>
+        <v>9392.679911349</v>
       </c>
       <c r="E16">
-        <v>0.379709182012551</v>
+        <v>1.19542038366041</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1">
-        <v>3945821.66126106</v>
+        <v>4329739.01448522</v>
       </c>
       <c r="B17">
-        <v>981</v>
+        <v>3028</v>
       </c>
       <c r="C17">
-        <v>1022.55334345391</v>
+        <v>482.568259644277</v>
       </c>
       <c r="D17">
-        <v>4746.71882962853</v>
+        <v>9625.96539612402</v>
       </c>
       <c r="E17">
-        <v>0.306272566393438</v>
+        <v>0.6894761958834</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1">
-        <v>3951293.4769674</v>
+        <v>4378501.54664203</v>
       </c>
       <c r="B18">
-        <v>1416</v>
+        <v>2888</v>
       </c>
       <c r="C18">
-        <v>887.678195705465</v>
+        <v>763.247022158778</v>
       </c>
       <c r="D18">
-        <v>2894.76857229332</v>
+        <v>7642.11631616895</v>
       </c>
       <c r="E18">
-        <v>0.243037710063721</v>
+        <v>1.43120140159059</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1">
-        <v>3975229.8266604</v>
+        <v>4401134.15871776</v>
       </c>
       <c r="B19">
-        <v>1593</v>
+        <v>2873</v>
       </c>
       <c r="C19">
-        <v>887.678195705465</v>
+        <v>721.694732934602</v>
       </c>
       <c r="D19">
-        <v>7492.24125491284</v>
+        <v>9278.44259673053</v>
       </c>
       <c r="E19">
-        <v>0.456523638807873</v>
+        <v>1.18912870775453</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1">
-        <v>3981895.49968627</v>
+        <v>4410716.7692045</v>
       </c>
       <c r="B20">
-        <v>1574</v>
+        <v>240</v>
       </c>
       <c r="C20">
-        <v>887.678195705465</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D20">
-        <v>7492.24125491284</v>
+        <v>30372.6270680987</v>
       </c>
       <c r="E20">
-        <v>0.453792091695951</v>
+        <v>1.29900527906299</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1">
-        <v>4001755.64759241</v>
+        <v>4411033.17908504</v>
       </c>
       <c r="B21">
-        <v>1539</v>
+        <v>240</v>
       </c>
       <c r="C21">
-        <v>887.678195705465</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D21">
-        <v>7492.24125491284</v>
+        <v>33220.3159929285</v>
       </c>
       <c r="E21">
-        <v>0.450133036232049</v>
+        <v>1.41648970014674</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1">
-        <v>4055362.20656925</v>
+        <v>4411098.49492872</v>
       </c>
       <c r="B22">
-        <v>1612</v>
+        <v>243</v>
       </c>
       <c r="C22">
-        <v>887.678195705465</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D22">
-        <v>7492.24125491284</v>
+        <v>34801.3927199067</v>
       </c>
       <c r="E22">
-        <v>0.486890017457043</v>
+        <v>1.4841666418863</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1">
-        <v>4091127.84600012</v>
+        <v>4411120.07968002</v>
       </c>
       <c r="B23">
-        <v>1593</v>
+        <v>240</v>
       </c>
       <c r="C23">
-        <v>1030.42427675926</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D23">
-        <v>7492.24125491284</v>
+        <v>34002.4213477483</v>
       </c>
       <c r="E23">
-        <v>0.683864423136252</v>
+        <v>1.44875984861564</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1">
-        <v>4092589.44264201</v>
+        <v>4411284.9891998</v>
       </c>
       <c r="B24">
-        <v>1630</v>
+        <v>240</v>
       </c>
       <c r="C24">
-        <v>1022.55334345391</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D24">
-        <v>6947.21541881574</v>
+        <v>35486.6070257827</v>
       </c>
       <c r="E24">
-        <v>0.680433787379498</v>
+        <v>1.51000248704163</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1">
-        <v>4109135.4404287</v>
+        <v>4411407.07921178</v>
       </c>
       <c r="B25">
-        <v>1480</v>
+        <v>240</v>
       </c>
       <c r="C25">
-        <v>1042.58143201635</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D25">
-        <v>4661.09651272204</v>
+        <v>36585.4171336441</v>
       </c>
       <c r="E25">
-        <v>0.509340179430123</v>
+        <v>1.55534675973653</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1">
-        <v>4127948.85059729</v>
+        <v>4411523.53179068</v>
       </c>
       <c r="B26">
-        <v>1371</v>
+        <v>240</v>
       </c>
       <c r="C26">
-        <v>887.678195705465</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D26">
-        <v>7492.24125491284</v>
+        <v>37633.4903437089</v>
       </c>
       <c r="E26">
-        <v>0.435995789566872</v>
+        <v>1.59860011380155</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1">
-        <v>4150089.9903169</v>
+        <v>4414666.77426179</v>
       </c>
       <c r="B27">
-        <v>2168</v>
+        <v>188</v>
       </c>
       <c r="C27">
-        <v>887.678195705465</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D27">
-        <v>10446.966014536</v>
+        <v>34584.6332283952</v>
       </c>
       <c r="E27">
-        <v>0.779116761379869</v>
+        <v>1.43197483761102</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1">
-        <v>4166559.99428197</v>
+        <v>4416092.77410753</v>
       </c>
       <c r="B28">
-        <v>858</v>
+        <v>188</v>
       </c>
       <c r="C28">
-        <v>1059.92178896587</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D28">
-        <v>1419.25840163854</v>
+        <v>47418.6318400049</v>
       </c>
       <c r="E28">
-        <v>0.150874356645709</v>
+        <v>1.94721815739368</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1">
-        <v>4184908.7081319</v>
+        <v>4417891.51203157</v>
       </c>
       <c r="B29">
-        <v>294</v>
+        <v>240</v>
       </c>
       <c r="C29">
-        <v>1059.92178896587</v>
+        <v>1103.05082236388</v>
       </c>
       <c r="D29">
-        <v>1419.25840163854</v>
+        <v>32445.4542497048</v>
       </c>
       <c r="E29">
-        <v>0.101084163498593</v>
+        <v>1.40062360819189</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1">
-        <v>4236396.52508314</v>
+        <v>4419659.45637617</v>
       </c>
       <c r="B30">
-        <v>1518</v>
+        <v>2916</v>
       </c>
       <c r="C30">
-        <v>724.445611661838</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D30">
-        <v>6295.92737192077</v>
+        <v>6574.80903910942</v>
       </c>
       <c r="E30">
-        <v>0.320556693683452</v>
+        <v>0.710421797663215</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1">
-        <v>4311295.80791395</v>
+        <v>4426884.5003455</v>
       </c>
       <c r="B31">
-        <v>1185</v>
+        <v>124</v>
       </c>
       <c r="C31">
-        <v>887.678195705465</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D31">
-        <v>7492.24125491284</v>
+        <v>58423.0872824849</v>
       </c>
       <c r="E31">
-        <v>0.426592186249258</v>
+        <v>2.31078828776659</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1">
-        <v>4355763.28015706</v>
+        <v>4427572.53832114</v>
       </c>
       <c r="B32">
-        <v>2367</v>
+        <v>124</v>
       </c>
       <c r="C32">
-        <v>919.254061093366</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D32">
-        <v>12506.0475554062</v>
+        <v>64615.429063215</v>
       </c>
       <c r="E32">
-        <v>1.11944627393133</v>
+        <v>2.55155379408215</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1">
-        <v>4396171.51981923</v>
+        <v>4428158.87822586</v>
       </c>
       <c r="B33">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="C33">
-        <v>1059.92178896587</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D33">
-        <v>144.850082077046</v>
+        <v>69892.4882057386</v>
       </c>
       <c r="E33">
-        <v>0.0445597759946305</v>
+        <v>2.75679948751535</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1">
-        <v>4399750.47367059</v>
+        <v>4428727.74391934</v>
       </c>
       <c r="B34">
-        <v>187</v>
+        <v>124</v>
       </c>
       <c r="C34">
-        <v>1059.92178896587</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D34">
-        <v>4027.11482883467</v>
+        <v>75012.2794470277</v>
       </c>
       <c r="E34">
-        <v>0.197873870477752</v>
+        <v>2.95598775800568</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1">
-        <v>4402383.15149808</v>
+        <v>4449480.44658224</v>
       </c>
       <c r="B35">
-        <v>472</v>
+        <v>36</v>
       </c>
       <c r="C35">
-        <v>1059.92178896587</v>
+        <v>1093.38080932301</v>
       </c>
       <c r="D35">
-        <v>32742.705613396</v>
+        <v>38431.1903502174</v>
       </c>
       <c r="E35">
-        <v>1.53045923374762</v>
+        <v>1.46748505572557</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1">
-        <v>4402403.31990608</v>
+        <v>4475422.04167998</v>
       </c>
       <c r="B36">
-        <v>187</v>
+        <v>2873</v>
       </c>
       <c r="C36">
-        <v>1059.92178896587</v>
+        <v>645.543807179659</v>
       </c>
       <c r="D36">
-        <v>49329.7678610463</v>
+        <v>10760.4427860563</v>
       </c>
       <c r="E36">
-        <v>1.94805360922766</v>
+        <v>0.963329300639201</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1">
-        <v>4402423.32207524</v>
+        <v>4481316.37177146</v>
       </c>
       <c r="B37">
-        <v>1795</v>
+        <v>200</v>
       </c>
       <c r="C37">
-        <v>654.892258996827</v>
+        <v>1167.42645400832</v>
       </c>
       <c r="D37">
-        <v>7492.24125491284</v>
+        <v>34436.7052332723</v>
       </c>
       <c r="E37">
-        <v>0.384444010980056</v>
+        <v>1.57016960703647</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1">
-        <v>4419808.54431656</v>
+        <v>4495749.94312634</v>
       </c>
       <c r="B38">
-        <v>563</v>
+        <v>240</v>
       </c>
       <c r="C38">
-        <v>1059.92178896587</v>
+        <v>1177.50874360641</v>
       </c>
       <c r="D38">
-        <v>29469.0999955439</v>
+        <v>31414.7256537485</v>
       </c>
       <c r="E38">
-        <v>1.46238589262288</v>
+        <v>1.49089737299565</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1">
-        <v>4429707.31388593</v>
+        <v>4561518.81549609</v>
       </c>
       <c r="B39">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="C39">
-        <v>1059.92178896587</v>
+        <v>1226.68187832501</v>
       </c>
       <c r="D39">
-        <v>14638.3198062041</v>
+        <v>34584.6332283952</v>
       </c>
       <c r="E39">
-        <v>0.574126098860063</v>
+        <v>1.51925664753212</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1">
-        <v>4429992.34772388</v>
+        <v>4569681.75456036</v>
       </c>
       <c r="B40">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="C40">
-        <v>1059.92178896587</v>
+        <v>942.066045909237</v>
       </c>
       <c r="D40">
-        <v>12073.015264593</v>
+        <v>45625.7132450043</v>
       </c>
       <c r="E40">
-        <v>0.480373734378998</v>
+        <v>1.55140008972025</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1">
-        <v>4430182.34783271</v>
+        <v>4605917.42310122</v>
       </c>
       <c r="B41">
-        <v>76</v>
+        <v>3618</v>
       </c>
       <c r="C41">
-        <v>1059.92178896587</v>
+        <v>670.296872296918</v>
       </c>
       <c r="D41">
-        <v>10363.0142851701</v>
+        <v>9392.679911349</v>
       </c>
       <c r="E41">
-        <v>0.41788674800364</v>
+        <v>3.25429761282742</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1">
-        <v>4430650.83166514</v>
+        <v>4705133.05938894</v>
       </c>
       <c r="B42">
-        <v>76</v>
+        <v>3493</v>
       </c>
       <c r="C42">
-        <v>1059.92178896587</v>
+        <v>456.963376410543</v>
       </c>
       <c r="D42">
-        <v>5156.84011618024</v>
+        <v>8138.57403593693</v>
       </c>
       <c r="E42">
-        <v>0.227709479905703</v>
+        <v>1.04079439099748</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1">
-        <v>4430865.32138658</v>
+        <v>4723460.9261716</v>
       </c>
       <c r="B43">
-        <v>76</v>
+        <v>2971</v>
       </c>
       <c r="C43">
-        <v>1059.92178896587</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D43">
-        <v>6122.0438626754</v>
+        <v>5433.17315478255</v>
       </c>
       <c r="E43">
-        <v>0.262981168719897</v>
+        <v>0.740376010754638</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1">
-        <v>4431179.79818744</v>
+        <v>4737452.75922526</v>
       </c>
       <c r="B44">
-        <v>76</v>
+        <v>2906</v>
       </c>
       <c r="C44">
-        <v>1062.42949211362</v>
+        <v>670.296872296918</v>
       </c>
       <c r="D44">
-        <v>8112.36006238842</v>
+        <v>12106.9723235305</v>
       </c>
       <c r="E44">
-        <v>0.336684859648634</v>
+        <v>1.07159659719616</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1">
-        <v>4487635.41502362</v>
+        <v>4744536.79653344</v>
       </c>
       <c r="B45">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="C45">
-        <v>1170.86029027366</v>
+        <v>1333.90925920213</v>
       </c>
       <c r="D45">
-        <v>4072.41982372247</v>
+        <v>51811.1993101071</v>
       </c>
       <c r="E45">
-        <v>0.216861295244407</v>
+        <v>2.797722403571</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1">
-        <v>4563543.2491971</v>
+        <v>4759581.68676397</v>
       </c>
       <c r="B46">
-        <v>1185</v>
+        <v>2242</v>
       </c>
       <c r="C46">
-        <v>1419.44464433334</v>
+        <v>233.11231800114</v>
       </c>
       <c r="D46">
-        <v>7492.24125491284</v>
+        <v>4922.74160935236</v>
       </c>
       <c r="E46">
-        <v>1.27470080136736</v>
+        <v>0.214573952399839</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1">
-        <v>4585262.14318462</v>
+        <v>4764444.65057091</v>
       </c>
       <c r="B47">
-        <v>1330</v>
+        <v>3618</v>
       </c>
       <c r="C47">
-        <v>1383.03326225539</v>
+        <v>670.296872296918</v>
       </c>
       <c r="D47">
-        <v>7725.51355470638</v>
+        <v>10564.8736708293</v>
       </c>
       <c r="E47">
-        <v>1.52373080528843</v>
+        <v>4.31460772890995</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1">
-        <v>4621188.84329052</v>
+        <v>4795857.82631817</v>
       </c>
       <c r="B48">
-        <v>1698</v>
+        <v>3304</v>
       </c>
       <c r="C48">
-        <v>887.678195705465</v>
+        <v>670.296872296918</v>
       </c>
       <c r="D48">
-        <v>11468.2569654453</v>
+        <v>11658.5095296316</v>
       </c>
       <c r="E48">
-        <v>0.878904637589424</v>
+        <v>1.88825736137206</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1">
-        <v>4679247.04777807</v>
+        <v>4965091.20172115</v>
       </c>
       <c r="B49">
-        <v>1480</v>
+        <v>3973</v>
       </c>
       <c r="C49">
-        <v>464.75237743133</v>
+        <v>298.638703602274</v>
       </c>
       <c r="D49">
-        <v>1811.52218048035</v>
+        <v>9570.48274779684</v>
       </c>
       <c r="E49">
-        <v>0.0978179459203013</v>
+        <v>1.17676014660975</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1">
-        <v>4681189.28274474</v>
+        <v>5109346.80955441</v>
       </c>
       <c r="B50">
-        <v>1185</v>
+        <v>2242</v>
       </c>
       <c r="C50">
-        <v>1020.40855313595</v>
+        <v>138.855177562764</v>
       </c>
       <c r="D50">
-        <v>23285.5395563521</v>
+        <v>3141.67509678102</v>
       </c>
       <c r="E50">
-        <v>1.76702030961274</v>
+        <v>0.139404258844564</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1">
-        <v>4705196.6795452</v>
+        <v>5109773.20587034</v>
       </c>
       <c r="B51">
-        <v>76</v>
+        <v>2971</v>
       </c>
       <c r="C51">
-        <v>1400.31134328679</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D51">
-        <v>583.526320006844</v>
+        <v>3866.76463402919</v>
       </c>
       <c r="E51">
-        <v>0.111290027227179</v>
+        <v>0.734606194391685</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1">
-        <v>4827941.01567751</v>
+        <v>5208067.69238724</v>
       </c>
       <c r="B52">
-        <v>1601</v>
+        <v>3367</v>
       </c>
       <c r="C52">
-        <v>1022.55334345391</v>
+        <v>571.91932337831</v>
       </c>
       <c r="D52">
-        <v>13146.5045121079</v>
+        <v>14814.3515858637</v>
       </c>
       <c r="E52">
-        <v>1.46013344308167</v>
+        <v>1.15435464439492</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1">
-        <v>4842319.90822489</v>
+        <v>5313550.23841531</v>
       </c>
       <c r="B53">
-        <v>1371</v>
+        <v>9</v>
       </c>
       <c r="C53">
-        <v>887.678195705465</v>
+        <v>809.728879588371</v>
       </c>
       <c r="D53">
-        <v>21479.9509052628</v>
+        <v>40768.4315206943</v>
       </c>
       <c r="E53">
-        <v>1.49201760451435</v>
+        <v>1.17883220593929</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1">
-        <v>4856249.11343424</v>
+        <v>5381371.12945544</v>
       </c>
       <c r="B54">
-        <v>76</v>
+        <v>2242</v>
       </c>
       <c r="C54">
-        <v>1420.38089762217</v>
+        <v>233.11231800114</v>
       </c>
       <c r="D54">
-        <v>144.850082077046</v>
+        <v>8027.68248046642</v>
       </c>
       <c r="E54">
-        <v>0.0916713870144583</v>
+        <v>0.319843811205614</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1">
-        <v>5047533.31552236</v>
+        <v>5415514.59598772</v>
       </c>
       <c r="B55">
-        <v>1593</v>
+        <v>2319</v>
       </c>
       <c r="C55">
-        <v>887.678195705465</v>
+        <v>868.145479701199</v>
       </c>
       <c r="D55">
-        <v>17972.0248722281</v>
+        <v>1068.10090375683</v>
       </c>
       <c r="E55">
-        <v>1.56449953342368</v>
+        <v>0.636496495126169</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1">
-        <v>5050683.00139636</v>
+        <v>5434083.1161573</v>
       </c>
       <c r="B56">
-        <v>2098</v>
+        <v>1551</v>
       </c>
       <c r="C56">
-        <v>1230.67437703912</v>
+        <v>233.11231800114</v>
       </c>
       <c r="D56">
-        <v>3787.95076128901</v>
+        <v>698.901146785603</v>
       </c>
       <c r="E56">
-        <v>-3.26169264889692</v>
+        <v>0.0405359341219319</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1">
-        <v>5123424.69653391</v>
+        <v>5517252.68740367</v>
       </c>
       <c r="B57">
-        <v>1509</v>
+        <v>5938</v>
       </c>
       <c r="C57">
-        <v>617.184673736136</v>
+        <v>0.692878390705573</v>
       </c>
       <c r="D57">
-        <v>9501.94560063691</v>
+        <v>18920.9093617079</v>
       </c>
       <c r="E57">
-        <v>0.4978031632626</v>
+        <v>2.75375419013127</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1">
-        <v>5186383.44961017</v>
+        <v>5682259.03608338</v>
       </c>
       <c r="B58">
-        <v>187</v>
+        <v>1551</v>
       </c>
       <c r="C58">
-        <v>756.588748702726</v>
+        <v>233.11231800114</v>
       </c>
       <c r="D58">
-        <v>39579.2737152571</v>
+        <v>27377.5716567773</v>
       </c>
       <c r="E58">
-        <v>1.17276718386234</v>
+        <v>0.894812472254449</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1">
-        <v>5186521.89816752</v>
+        <v>5683179.13488886</v>
       </c>
       <c r="B59">
-        <v>76</v>
+        <v>1551</v>
       </c>
       <c r="C59">
-        <v>808.117094388664</v>
+        <v>233.11231800114</v>
       </c>
       <c r="D59">
-        <v>2748.89573281135</v>
+        <v>35658.4609060607</v>
       </c>
       <c r="E59">
-        <v>0.10370172236113</v>
+        <v>1.16009941826007</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1">
-        <v>5298166.89589275</v>
+        <v>5719686.74400591</v>
       </c>
       <c r="B60">
-        <v>1371</v>
+        <v>5219</v>
       </c>
       <c r="C60">
-        <v>1392.51925224192</v>
+        <v>145.026423472807</v>
       </c>
       <c r="D60">
-        <v>14384.0470157332</v>
+        <v>12106.9723235305</v>
       </c>
       <c r="E60">
-        <v>5.22241952377792</v>
+        <v>7.00326138742145</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1">
-        <v>5344343.61586925</v>
+        <v>5732747.46478962</v>
       </c>
       <c r="B61">
-        <v>100</v>
+        <v>1801</v>
       </c>
       <c r="C61">
-        <v>1761.9304137062</v>
+        <v>275.08386406128</v>
       </c>
       <c r="D61">
-        <v>1990.63938430488</v>
+        <v>21786.3418634605</v>
       </c>
       <c r="E61">
-        <v>0.46530577032213</v>
+        <v>0.838757558658306</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1">
-        <v>5464525.91835947</v>
+        <v>5773837.30927491</v>
       </c>
       <c r="B62">
-        <v>194</v>
+        <v>1429</v>
       </c>
       <c r="C62">
-        <v>687.445305020189</v>
+        <v>1428.57142857143</v>
       </c>
       <c r="D62">
-        <v>7725.51355470638</v>
+        <v>42857.1428571429</v>
       </c>
       <c r="E62">
-        <v>0.232947699742726</v>
+        <v>-55.7745261705267</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1">
-        <v>5516509.51571414</v>
+        <v>5876081.94767828</v>
       </c>
       <c r="B63">
-        <v>1596</v>
+        <v>188</v>
       </c>
       <c r="C63">
-        <v>1747.37543118101</v>
+        <v>1781.10772581572</v>
       </c>
       <c r="D63">
-        <v>11344.8074227475</v>
+        <v>22804.8518494315</v>
       </c>
       <c r="E63">
-        <v>-3.06066431566642</v>
+        <v>4.39418353584179</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1">
-        <v>5544749.31269568</v>
+        <v>5876576.13728</v>
       </c>
       <c r="B64">
-        <v>1330</v>
+        <v>1378</v>
       </c>
       <c r="C64">
-        <v>1383.03326225539</v>
+        <v>148.21643105674</v>
       </c>
       <c r="D64">
-        <v>16276.1650991837</v>
+        <v>47039.1256955449</v>
       </c>
       <c r="E64">
-        <v>9.96362021549916</v>
+        <v>1.32335031123499</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1">
-        <v>5563329.4667058</v>
+        <v>5973375.04169834</v>
       </c>
       <c r="B65">
-        <v>1593</v>
+        <v>188</v>
       </c>
       <c r="C65">
-        <v>310.154285131011</v>
+        <v>2239.54160272784</v>
       </c>
       <c r="D65">
-        <v>7492.24125491284</v>
+        <v>9233.98435287439</v>
       </c>
       <c r="E65">
-        <v>0.285875240145995</v>
+        <v>-24.7426546214822</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1">
-        <v>5565624.92427213</v>
+        <v>6059783.99473311</v>
       </c>
       <c r="B66">
-        <v>194</v>
+        <v>4276</v>
       </c>
       <c r="C66">
-        <v>1897.8015614372</v>
+        <v>32.9082291056236</v>
       </c>
       <c r="D66">
-        <v>4364.21909728853</v>
+        <v>6537.76878879089</v>
       </c>
       <c r="E66">
-        <v>1.5130895835982</v>
+        <v>0.830160290242022</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1">
-        <v>5758006.86820518</v>
+        <v>6180878.67248843</v>
       </c>
       <c r="B67">
-        <v>2460</v>
+        <v>1244</v>
       </c>
       <c r="C67">
-        <v>1383.03326225539</v>
+        <v>1632.79980197472</v>
       </c>
       <c r="D67">
-        <v>5414.34255839407</v>
+        <v>31386.7007356822</v>
       </c>
       <c r="E67">
-        <v>-0.757334786685979</v>
+        <v>-8.10920859814484</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1">
-        <v>5772023.2664924</v>
+        <v>6271795.46813503</v>
       </c>
       <c r="B68">
-        <v>1429</v>
+        <v>188</v>
       </c>
       <c r="C68">
-        <v>1428.57142857143</v>
+        <v>499.260292963652</v>
       </c>
       <c r="D68">
-        <v>26530.7578146081</v>
+        <v>13894.8292687045</v>
       </c>
       <c r="E68">
-        <v>-35.9001837908512</v>
+        <v>0.346394171459145</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1">
-        <v>5778599.21403681</v>
+        <v>6297483.93565483</v>
       </c>
       <c r="B69">
-        <v>1429</v>
+        <v>188</v>
       </c>
       <c r="C69">
-        <v>1428.57142857143</v>
+        <v>493.38696384363</v>
       </c>
       <c r="D69">
-        <v>85714.2857142857</v>
+        <v>28332.4373358569</v>
       </c>
       <c r="E69">
-        <v>-105.203051241113</v>
+        <v>0.690129334640067</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1">
-        <v>5907727.54343101</v>
+        <v>6307266.5382834</v>
       </c>
       <c r="B70">
-        <v>1857</v>
+        <v>2906</v>
       </c>
       <c r="C70">
-        <v>188.710726000239</v>
+        <v>5.03574010021498</v>
       </c>
       <c r="D70">
-        <v>80877.8381101355</v>
+        <v>12106.9723235305</v>
       </c>
       <c r="E70">
-        <v>2.86594157291208</v>
+        <v>0.487247679246801</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1">
-        <v>5930991.98807065</v>
+        <v>6524728.22615845</v>
       </c>
       <c r="B71">
-        <v>848</v>
+        <v>2906</v>
       </c>
       <c r="C71">
-        <v>276.385920223578</v>
+        <v>1417.87229003004</v>
       </c>
       <c r="D71">
-        <v>11113.1527958468</v>
+        <v>12795.606682123</v>
       </c>
       <c r="E71">
-        <v>0.294799219799247</v>
+        <v>-1.08780338884876</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="1">
-        <v>5933896.41416396</v>
+        <v>6725913.98945829</v>
       </c>
       <c r="B72">
-        <v>848</v>
+        <v>47</v>
       </c>
       <c r="C72">
-        <v>276.385920223578</v>
+        <v>457.798283588894</v>
       </c>
       <c r="D72">
-        <v>50376.9658980047</v>
+        <v>18546.0655010668</v>
       </c>
       <c r="E72">
-        <v>1.2954927284771</v>
+        <v>0.425465507474859</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1">
-        <v>5938618.3693962</v>
+        <v>6871751.80912801</v>
       </c>
       <c r="B73">
-        <v>848</v>
+        <v>2852</v>
       </c>
       <c r="C73">
-        <v>276.385920223578</v>
+        <v>605.77556858584</v>
       </c>
       <c r="D73">
-        <v>92874.5629880678</v>
+        <v>89890.5377962267</v>
       </c>
       <c r="E73">
-        <v>2.38027109774279</v>
+        <v>25.2110402324289</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1">
-        <v>6190446.83733387</v>
+        <v>7106594.46790063</v>
       </c>
       <c r="B74">
-        <v>848</v>
+        <v>406</v>
       </c>
       <c r="C74">
-        <v>211.643385611146</v>
+        <v>200.238362838399</v>
       </c>
       <c r="D74">
-        <v>69654.0386078533</v>
+        <v>15147.1336834127</v>
       </c>
       <c r="E74">
-        <v>1.70645731302293</v>
+        <v>0.326917123915005</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1">
-        <v>6225259.59785632</v>
+        <v>7114319.42390906</v>
       </c>
       <c r="B75">
-        <v>848</v>
+        <v>2906</v>
       </c>
       <c r="C75">
-        <v>202.383213359027</v>
+        <v>208.611725633205</v>
       </c>
       <c r="D75">
-        <v>36016.7939122223</v>
+        <v>32019.5002425451</v>
       </c>
       <c r="E75">
-        <v>0.880735746058059</v>
+        <v>2.32791289873551</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1">
-        <v>6285841.32791764</v>
+        <v>7115299.66768362</v>
       </c>
       <c r="B76">
-        <v>194</v>
+        <v>2906</v>
       </c>
       <c r="C76">
-        <v>493.397830410191</v>
+        <v>204.632317584283</v>
       </c>
       <c r="D76">
-        <v>30754.4317825477</v>
+        <v>19055.6412588232</v>
       </c>
       <c r="E76">
-        <v>0.74951368031002</v>
+        <v>1.39758839715531</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1">
-        <v>6328044.5209312</v>
+        <v>7146193.23380673</v>
       </c>
       <c r="B77">
-        <v>1185</v>
+        <v>188</v>
       </c>
       <c r="C77">
-        <v>1984.11704244766</v>
+        <v>2195.64759730576</v>
       </c>
       <c r="D77">
-        <v>6029.82484098493</v>
+        <v>34584.6332283952</v>
       </c>
       <c r="E77">
-        <v>-0.79013492125824</v>
+        <v>-6.06950092988319</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="1">
-        <v>6353830.77360606</v>
+        <v>7170133.65821767</v>
       </c>
       <c r="B78">
-        <v>1211</v>
+        <v>3618</v>
       </c>
       <c r="C78">
-        <v>22.3406250290276</v>
+        <v>670.296872296918</v>
       </c>
       <c r="D78">
-        <v>12764.0507670268</v>
+        <v>1634.53052958511</v>
       </c>
       <c r="E78">
-        <v>0.313456715690685</v>
+        <v>-0.421557533937506</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1">
-        <v>6616335.49727413</v>
+        <v>7300714.23090214</v>
       </c>
       <c r="B79">
-        <v>2744</v>
+        <v>3618</v>
       </c>
       <c r="C79">
-        <v>276.385920223578</v>
+        <v>670.296872296918</v>
       </c>
       <c r="D79">
-        <v>349.446223005227</v>
+        <v>25028.3770172878</v>
       </c>
       <c r="E79">
-        <v>0.0855712097817007</v>
+        <v>-11.2261099425898</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1">
-        <v>6701690.28289095</v>
+        <v>7532473.80853621</v>
       </c>
       <c r="B80">
-        <v>328</v>
+        <v>124</v>
       </c>
       <c r="C80">
-        <v>333.321466140762</v>
+        <v>233.006677256502</v>
       </c>
       <c r="D80">
-        <v>58908.7229157766</v>
+        <v>82692.5547611731</v>
       </c>
       <c r="E80">
-        <v>1.33381145362988</v>
+        <v>1.66053426320143</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1">
-        <v>6969819.7683523</v>
+        <v>7597763.98952276</v>
       </c>
       <c r="B81">
-        <v>1185</v>
+        <v>88</v>
       </c>
       <c r="C81">
-        <v>2057.69451022518</v>
+        <v>233.11231800114</v>
       </c>
       <c r="D81">
-        <v>1985.40559940985</v>
+        <v>935.488333725212</v>
       </c>
       <c r="E81">
-        <v>-0.294983759978639</v>
+        <v>0.0235346271730997</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1">
-        <v>7033622.10134314</v>
+        <v>7708712.3328352</v>
       </c>
       <c r="B82">
-        <v>848</v>
+        <v>511</v>
       </c>
       <c r="C82">
-        <v>11.140808504107</v>
+        <v>9.79779887963196</v>
       </c>
       <c r="D82">
-        <v>25290.116648554</v>
+        <v>51811.1993101071</v>
       </c>
       <c r="E82">
-        <v>0.545513529740776</v>
+        <v>1.01488723294884</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1">
-        <v>7250429.94655382</v>
+        <v>8157800.28912984</v>
       </c>
       <c r="B83">
-        <v>693</v>
+        <v>124</v>
       </c>
       <c r="C83">
-        <v>32.3838284031814</v>
+        <v>2514.13962767432</v>
       </c>
       <c r="D83">
-        <v>4352.25585142569</v>
+        <v>56873.7299470038</v>
       </c>
       <c r="E83">
-        <v>0.0942066423737323</v>
+        <v>-4.18341000120861</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1">
-        <v>7375021.47133481</v>
+        <v>8289222.8700003</v>
       </c>
       <c r="B84">
-        <v>520</v>
+        <v>188</v>
       </c>
       <c r="C84">
-        <v>83.6990977593632</v>
+        <v>23.1066556020669</v>
       </c>
       <c r="D84">
-        <v>11113.1527958468</v>
+        <v>34584.6332283952</v>
       </c>
       <c r="E84">
-        <v>0.230840140768277</v>
+        <v>0.629356045543313</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="1">
-        <v>7561325.43268305</v>
+        <v>8989536.86012849</v>
       </c>
       <c r="B85">
-        <v>13</v>
+        <v>2912</v>
       </c>
       <c r="C85">
-        <v>276.385920223578</v>
+        <v>2193.40415388584</v>
       </c>
       <c r="D85">
-        <v>19623.791406405</v>
+        <v>17364.2293111359</v>
       </c>
       <c r="E85">
-        <v>0.396156248795336</v>
+        <v>-0.582750412437883</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="1">
-        <v>8375517.1272429</v>
+        <v>9343466.95209284</v>
       </c>
       <c r="B86">
-        <v>187</v>
+        <v>2486</v>
       </c>
       <c r="C86">
-        <v>2.80141864429834</v>
+        <v>2460.32942747984</v>
       </c>
       <c r="D86">
-        <v>19730.6541487943</v>
+        <v>9476.55767949854</v>
       </c>
       <c r="E86">
-        <v>0.355340464954804</v>
+        <v>-0.316566772493463</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="1">
-        <v>8548047.0829247</v>
+        <v>15540147.6783496</v>
       </c>
       <c r="B87">
-        <v>76</v>
+        <v>4286</v>
       </c>
       <c r="C87">
-        <v>14.3178321799519</v>
+        <v>2857.14285714286</v>
       </c>
       <c r="D87">
-        <v>144.850082077046</v>
+        <v>71428.5714285714</v>
       </c>
       <c r="E87">
-        <v>0.00309959881674946</v>
+        <v>-0.957769729506927</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="1">
-        <v>10600774.1362006</v>
+        <v>16134399.8381406</v>
       </c>
       <c r="B88">
-        <v>1429</v>
+        <v>124</v>
       </c>
       <c r="C88">
-        <v>2857.14285714286</v>
+        <v>4668.20390762309</v>
       </c>
       <c r="D88">
-        <v>42857.1428571429</v>
+        <v>39523.8130558023</v>
       </c>
       <c r="E88">
-        <v>-1.12297102342341</v>
+        <v>-0.591232063986418</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="1">
-        <v>11625845.8157368</v>
+        <v>17864445.5203023</v>
       </c>
       <c r="B89">
-        <v>76</v>
+        <v>8921</v>
       </c>
       <c r="C89">
-        <v>3511.03380557672</v>
+        <v>233.11231800114</v>
       </c>
       <c r="D89">
-        <v>144.850082077046</v>
+        <v>515.437905060138</v>
       </c>
       <c r="E89">
-        <v>-0.0883484103113231</v>
+        <v>-0.0416567151758307</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="1">
-        <v>11706977.467638</v>
+        <v>18433533.6856317</v>
       </c>
       <c r="B90">
-        <v>7143</v>
+        <v>2857</v>
       </c>
       <c r="C90">
-        <v>1428.57142857143</v>
+        <v>4285.71428571429</v>
       </c>
       <c r="D90">
-        <v>14285.7142857143</v>
+        <v>85714.2857142857</v>
       </c>
       <c r="E90">
-        <v>-0.274088315524977</v>
+        <v>-0.906536631618195</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="1">
-        <v>16068694.1011575</v>
+        <v>18544103.5910568</v>
       </c>
       <c r="B91">
-        <v>2857</v>
+        <v>4286</v>
       </c>
       <c r="C91">
         <v>4285.71428571429</v>
@@ -1930,58 +1930,58 @@
         <v>28571.4285714286</v>
       </c>
       <c r="E91">
-        <v>-0.38096696124128</v>
+        <v>-0.318086106012612</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="1">
-        <v>20980668.1797636</v>
+        <v>20082975.1173336</v>
       </c>
       <c r="B92">
         <v>8571</v>
       </c>
       <c r="C92">
-        <v>7142.85714285714</v>
+        <v>2857.14285714286</v>
       </c>
       <c r="D92">
-        <v>85714.2857142857</v>
+        <v>14285.7142857143</v>
       </c>
       <c r="E92">
-        <v>-0.77603438027224</v>
+        <v>-0.151398394186692</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="1">
-        <v>21059325.0307752</v>
+        <v>21583881.3490185</v>
       </c>
       <c r="B93">
-        <v>7143</v>
+        <v>10000</v>
       </c>
       <c r="C93">
-        <v>2857.14285714286</v>
+        <v>1428.57142857143</v>
       </c>
       <c r="D93">
         <v>100000</v>
       </c>
       <c r="E93">
-        <v>-0.899452611618965</v>
+        <v>-0.913448231815579</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="1">
-        <v>23392513.0505901</v>
+        <v>22930832.1372871</v>
       </c>
       <c r="B94">
-        <v>2857</v>
+        <v>7143</v>
       </c>
       <c r="C94">
         <v>7142.85714285714</v>
       </c>
       <c r="D94">
-        <v>71428.5714285714</v>
+        <v>85714.2857142857</v>
       </c>
       <c r="E94">
-        <v>-0.580372579150286</v>
+        <v>-0.699984212172992</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2020,75 +2020,75 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="1">
-        <v>26486791.3739845</v>
+        <v>35884457.4834066</v>
       </c>
       <c r="B97">
-        <v>8571</v>
+        <v>2857</v>
       </c>
       <c r="C97">
-        <v>4285.71428571429</v>
+        <v>8571.42857142857</v>
       </c>
       <c r="D97">
-        <v>42857.1428571429</v>
+        <v>100000</v>
       </c>
       <c r="E97">
-        <v>-0.291197158597544</v>
+        <v>-0.495122856366093</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="1">
-        <v>30426872.7829687</v>
+        <v>37681377.2555752</v>
       </c>
       <c r="B98">
-        <v>4286</v>
+        <v>1429</v>
       </c>
       <c r="C98">
         <v>10000</v>
       </c>
       <c r="D98">
-        <v>100000</v>
+        <v>14285.7142857143</v>
       </c>
       <c r="E98">
-        <v>-0.596787324623685</v>
+        <v>-0.103446905397738</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="1">
-        <v>36594075.3097996</v>
+        <v>37974123.6271293</v>
       </c>
       <c r="B99">
-        <v>4286</v>
+        <v>8571</v>
       </c>
       <c r="C99">
-        <v>8571.42857142857</v>
+        <v>7142.85714285714</v>
       </c>
       <c r="D99">
-        <v>14285.7142857143</v>
+        <v>28571.4285714286</v>
       </c>
       <c r="E99">
-        <v>-0.101871991872319</v>
+        <v>-0.152205656468767</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="1">
-        <v>46547198.3150749</v>
+        <v>41749901.052711</v>
       </c>
       <c r="B100">
-        <v>10000</v>
+        <v>7143</v>
       </c>
       <c r="C100">
         <v>8571.42857142857</v>
       </c>
       <c r="D100">
-        <v>71428.5714285714</v>
+        <v>42857.1428571429</v>
       </c>
       <c r="E100">
-        <v>-0.271340589291061</v>
+        <v>-0.191937901488258</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="1">
-        <v>52681085.6381219</v>
+        <v>53388954.4741442</v>
       </c>
       <c r="B101">
         <v>10000</v>
@@ -2097,10 +2097,10 @@
         <v>10000</v>
       </c>
       <c r="D101">
-        <v>28571.4285714286</v>
+        <v>71428.5714285714</v>
       </c>
       <c r="E101">
-        <v>-0.117533417230242</v>
+        <v>-0.237345951492068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>